<commit_message>
final work; q1 working
</commit_message>
<xml_diff>
--- a/final/q1-output.xlsx
+++ b/final/q1-output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aelhabr\Documents\projects\isye-6420\final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFFFBE82-5599-41A2-85BB-72FD7B939957}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0532998B-CA72-4C89-A75B-5214B89F7228}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14220" yWindow="1875" windowWidth="12825" windowHeight="9345" xr2:uid="{FACCC27F-6028-4B1F-9F8A-BE4A2FC85474}"/>
+    <workbookView xWindow="14220" yWindow="1875" windowWidth="12825" windowHeight="9345" xr2:uid="{FB629626-7784-4A97-8620-D9E5DAF05A78}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,6 +66,18 @@
     <t>b2</t>
   </si>
   <si>
+    <t>mu1</t>
+  </si>
+  <si>
+    <t>mu2</t>
+  </si>
+  <si>
+    <t>pred1</t>
+  </si>
+  <si>
+    <t>pred2</t>
+  </si>
+  <si>
     <t>sigma</t>
   </si>
   <si>
@@ -73,18 +85,6 @@
   </si>
   <si>
     <t>var</t>
-  </si>
-  <si>
-    <t>mu1</t>
-  </si>
-  <si>
-    <t>mu2</t>
-  </si>
-  <si>
-    <t>pred1</t>
-  </si>
-  <si>
-    <t>pred2</t>
   </si>
 </sst>
 </file>
@@ -436,7 +436,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E133526-8219-499B-A85E-9B1090890EDA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F03859D-A37F-48CE-8DE5-8FD927FBA19B}">
   <dimension ref="B1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -445,7 +445,7 @@
   <sheetData>
     <row r="1" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
@@ -477,22 +477,22 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <v>2029</v>
+        <v>1009</v>
       </c>
       <c r="D2">
-        <v>31.61</v>
+        <v>25.28</v>
       </c>
       <c r="E2">
-        <v>2.6909999999999998</v>
+        <v>2.0070000000000001</v>
       </c>
       <c r="F2">
-        <v>1963</v>
+        <v>958</v>
       </c>
       <c r="G2">
-        <v>2029</v>
+        <v>1011</v>
       </c>
       <c r="H2">
-        <v>2087</v>
+        <v>1055</v>
       </c>
       <c r="I2">
         <v>1001</v>
@@ -506,22 +506,22 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>-44.62</v>
+        <v>-1.1919999999999999</v>
       </c>
       <c r="D3">
-        <v>1.351</v>
+        <v>1.087</v>
       </c>
       <c r="E3">
-        <v>0.11509999999999999</v>
+        <v>8.6319999999999994E-2</v>
       </c>
       <c r="F3">
-        <v>-47.07</v>
+        <v>-3.161</v>
       </c>
       <c r="G3">
-        <v>-44.64</v>
+        <v>-1.276</v>
       </c>
       <c r="H3">
-        <v>-41.81</v>
+        <v>1.006</v>
       </c>
       <c r="I3">
         <v>1001</v>
@@ -535,22 +535,22 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>-171.2</v>
       </c>
       <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="1">
-        <v>9.9999999999999998E-13</v>
+        <v>23.44</v>
+      </c>
+      <c r="E4">
+        <v>0.2167</v>
       </c>
       <c r="F4">
-        <v>0</v>
+        <v>-217</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>-171.3</v>
       </c>
       <c r="H4">
-        <v>0</v>
+        <v>-125.1</v>
       </c>
       <c r="I4">
         <v>1001</v>
@@ -561,25 +561,25 @@
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C5">
-        <v>957.8</v>
+        <v>980.2</v>
       </c>
       <c r="D5">
-        <v>3.3730000000000002</v>
+        <v>3.4569999999999999</v>
       </c>
       <c r="E5">
-        <v>7.9189999999999997E-2</v>
+        <v>7.3349999999999999E-2</v>
       </c>
       <c r="F5">
-        <v>951.2</v>
+        <v>973.4</v>
       </c>
       <c r="G5">
-        <v>957.8</v>
+        <v>980.2</v>
       </c>
       <c r="H5">
-        <v>964.4</v>
+        <v>987.1</v>
       </c>
       <c r="I5">
         <v>1001</v>
@@ -590,25 +590,25 @@
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C6">
-        <v>779.4</v>
+        <v>804.2</v>
       </c>
       <c r="D6">
-        <v>7.157</v>
+        <v>24.05</v>
       </c>
       <c r="E6">
-        <v>0.53339999999999999</v>
+        <v>0.46610000000000001</v>
       </c>
       <c r="F6">
-        <v>766</v>
+        <v>757</v>
       </c>
       <c r="G6">
-        <v>779.2</v>
+        <v>804.2</v>
       </c>
       <c r="H6">
-        <v>793.7</v>
+        <v>851.3</v>
       </c>
       <c r="I6">
         <v>1001</v>
@@ -619,25 +619,25 @@
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C7">
-        <v>956.9</v>
+        <v>975.7</v>
       </c>
       <c r="D7">
-        <v>410</v>
+        <v>429.9</v>
       </c>
       <c r="E7">
-        <v>4.0590000000000002</v>
+        <v>4.5469999999999997</v>
       </c>
       <c r="F7">
-        <v>143.4</v>
+        <v>142.80000000000001</v>
       </c>
       <c r="G7">
-        <v>960.9</v>
+        <v>973.6</v>
       </c>
       <c r="H7">
-        <v>1767</v>
+        <v>1835</v>
       </c>
       <c r="I7">
         <v>1001</v>
@@ -648,25 +648,25 @@
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C8">
-        <v>772.7</v>
+        <v>802.5</v>
       </c>
       <c r="D8">
-        <v>415.8</v>
+        <v>425.8</v>
       </c>
       <c r="E8">
-        <v>4.0880000000000001</v>
+        <v>4.1360000000000001</v>
       </c>
       <c r="F8">
-        <v>-41.72</v>
+        <v>-36.39</v>
       </c>
       <c r="G8">
-        <v>772.6</v>
+        <v>803.5</v>
       </c>
       <c r="H8">
-        <v>1580</v>
+        <v>1629</v>
       </c>
       <c r="I8">
         <v>1001</v>
@@ -677,25 +677,25 @@
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C9">
-        <v>411.4</v>
+        <v>426.5</v>
       </c>
       <c r="D9">
-        <v>2.2749999999999999</v>
+        <v>2.4529999999999998</v>
       </c>
       <c r="E9">
-        <v>2.4879999999999999E-2</v>
+        <v>5.9069999999999998E-2</v>
       </c>
       <c r="F9">
-        <v>407</v>
+        <v>421.8</v>
       </c>
       <c r="G9">
-        <v>411.4</v>
+        <v>426.5</v>
       </c>
       <c r="H9">
-        <v>415.9</v>
+        <v>431.3</v>
       </c>
       <c r="I9">
         <v>1001</v>
@@ -706,25 +706,25 @@
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C10" s="1">
-        <v>5.9089999999999997E-6</v>
+        <v>5.4979999999999997E-6</v>
       </c>
       <c r="D10" s="1">
-        <v>6.535E-8</v>
+        <v>6.3250000000000001E-8</v>
       </c>
       <c r="E10" s="1">
-        <v>7.143E-10</v>
+        <v>1.5239999999999999E-9</v>
       </c>
       <c r="F10" s="1">
-        <v>5.7819999999999999E-6</v>
+        <v>5.3759999999999999E-6</v>
       </c>
       <c r="G10" s="1">
-        <v>5.908E-6</v>
+        <v>5.4979999999999997E-6</v>
       </c>
       <c r="H10" s="1">
-        <v>6.0379999999999996E-6</v>
+        <v>5.6219999999999997E-6</v>
       </c>
       <c r="I10">
         <v>1001</v>

</xml_diff>